<commit_message>
Make 'mom' and 'dad' stopwords
</commit_message>
<xml_diff>
--- a/resources/WordCategories.xlsx
+++ b/resources/WordCategories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="0" windowWidth="21680" windowHeight="14400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3920" yWindow="0" windowWidth="21680" windowHeight="14380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="1038">
   <si>
     <t>Nouns</t>
   </si>
@@ -3606,7 +3606,7 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A481" sqref="A481"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -3703,8 +3703,8 @@
         <v>10</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f>COUNTA(K3:K479)</f>
+        <v>13</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" si="0"/>
@@ -3713,7 +3713,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="6">
         <f>SUM(A2:L2)</f>
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3818,7 +3818,7 @@
         <v>43</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>45</v>
@@ -3856,7 +3856,7 @@
         <v>55</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>57</v>
@@ -3890,8 +3890,8 @@
       <c r="J7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="K7" s="7" t="s">
-        <v>66</v>
+      <c r="K7" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="L7" s="7" t="s">
         <v>67</v>
@@ -3923,8 +3923,8 @@
       <c r="J8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>76</v>
+      <c r="K8" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>77</v>
@@ -3956,8 +3956,8 @@
       <c r="J9" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>86</v>
+      <c r="K9" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>87</v>
@@ -3989,8 +3989,8 @@
       <c r="J10" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>96</v>
+      <c r="K10" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="L10" s="7" t="s">
         <v>97</v>
@@ -4020,7 +4020,7 @@
         <v>104</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="L11" s="7" t="s">
         <v>106</v>
@@ -4050,7 +4050,7 @@
         <v>113</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -4074,7 +4074,7 @@
         <v>120</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -4094,8 +4094,8 @@
       <c r="F14" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="K14" s="8" t="s">
-        <v>127</v>
+      <c r="K14" s="7" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -4116,7 +4116,7 @@
         <v>132</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -4136,11 +4136,8 @@
       <c r="F16" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="K16" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="7" t="s">
         <v>140</v>
       </c>
@@ -4157,11 +4154,8 @@
       <c r="F17" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="K17" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="7" t="s">
         <v>146</v>
       </c>
@@ -4179,7 +4173,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:6">
       <c r="A19" s="7" t="s">
         <v>151</v>
       </c>
@@ -4197,7 +4191,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:6">
       <c r="A20" s="7" t="s">
         <v>156</v>
       </c>
@@ -4215,7 +4209,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:6">
       <c r="A21" s="7" t="s">
         <v>161</v>
       </c>
@@ -4233,7 +4227,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
         <v>166</v>
       </c>
@@ -4251,7 +4245,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
         <v>171</v>
       </c>
@@ -4269,7 +4263,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
         <v>176</v>
       </c>
@@ -4284,7 +4278,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:6">
       <c r="A25" s="7" t="s">
         <v>180</v>
       </c>
@@ -4299,7 +4293,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:6">
       <c r="A26" s="7" t="s">
         <v>183</v>
       </c>
@@ -4312,7 +4306,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:6">
       <c r="A27" s="7" t="s">
         <v>186</v>
       </c>
@@ -4325,7 +4319,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:6">
       <c r="A28" s="7" t="s">
         <v>189</v>
       </c>
@@ -4338,7 +4332,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:6">
       <c r="A29" s="7" t="s">
         <v>192</v>
       </c>
@@ -4351,7 +4345,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>195</v>
       </c>
@@ -4364,7 +4358,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:6">
       <c r="A31" s="8" t="s">
         <v>198</v>
       </c>
@@ -4377,7 +4371,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:6">
       <c r="A32" s="7" t="s">
         <v>201</v>
       </c>
@@ -12879,10 +12873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z70"/>
+  <dimension ref="A1:Z68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -12948,7 +12942,7 @@
       </c>
       <c r="F2" s="9">
         <f>COUNTA(A2:E98)</f>
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H2" s="9"/>
     </row>
@@ -13394,7 +13388,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="9" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>377</v>
@@ -13405,7 +13399,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="9" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>380</v>
@@ -13416,7 +13410,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="9" t="s">
-        <v>127</v>
+        <v>858</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>383</v>
@@ -13427,7 +13421,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="9" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>387</v>
@@ -13438,7 +13432,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="9" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>411</v>
@@ -13449,7 +13443,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="9" t="s">
-        <v>863</v>
+        <v>890</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>341</v>
@@ -13460,7 +13454,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="9" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>464</v>
@@ -13471,7 +13465,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="9" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>467</v>
@@ -13482,7 +13476,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="9" t="s">
-        <v>892</v>
+        <v>898</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>681</v>
@@ -13493,7 +13487,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="9" t="s">
-        <v>898</v>
+        <v>913</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>693</v>
@@ -13504,7 +13498,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="9" t="s">
-        <v>913</v>
+        <v>917</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>393</v>
@@ -13515,7 +13509,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="9" t="s">
-        <v>917</v>
+        <v>924</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>253</v>
@@ -13526,7 +13520,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="9" t="s">
-        <v>924</v>
+        <v>928</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>490</v>
@@ -13537,7 +13531,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="9" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>196</v>
@@ -13548,7 +13542,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="9" t="s">
-        <v>929</v>
+        <v>1019</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>608</v>
@@ -13556,7 +13550,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="9" t="s">
-        <v>1019</v>
+        <v>105</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>233</v>
@@ -13564,7 +13558,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="9" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>1020</v>
@@ -13572,7 +13566,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="9" t="s">
-        <v>96</v>
+        <v>649</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>287</v>
@@ -13580,7 +13574,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="9" t="s">
-        <v>44</v>
+        <v>1021</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>599</v>
@@ -13588,7 +13582,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="9" t="s">
-        <v>649</v>
+        <v>1022</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>764</v>
@@ -13596,7 +13590,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="9" t="s">
-        <v>1021</v>
+        <v>802</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>385</v>
@@ -13604,7 +13598,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="9" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>1023</v>
@@ -13612,7 +13606,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="9" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>1024</v>
@@ -13620,7 +13614,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="9" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>312</v>
@@ -13628,7 +13622,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="9" t="s">
-        <v>801</v>
+        <v>1028</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>637</v>
@@ -13636,7 +13630,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="9" t="s">
-        <v>1026</v>
+        <v>928</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>1027</v>
@@ -13644,7 +13638,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="9" t="s">
-        <v>1028</v>
+        <v>1031</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>1029</v>
@@ -13652,7 +13646,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="9" t="s">
-        <v>928</v>
+        <v>1032</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>1030</v>
@@ -13660,46 +13654,36 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="9" t="s">
-        <v>1031</v>
+        <v>935</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="9" t="s">
-        <v>1032</v>
+        <v>787</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="9" t="s">
-        <v>935</v>
+        <v>778</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="9" t="s">
-        <v>787</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="9" t="s">
-        <v>778</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="9" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="9" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="9" t="s">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="9" t="s">
         <v>1035</v>
       </c>
     </row>

</xml_diff>